<commit_message>
Improved costcenter select in compensations
</commit_message>
<xml_diff>
--- a/frontend/src/assets/comp mock.xlsx
+++ b/frontend/src/assets/comp mock.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Upplagd av</t>
   </si>
@@ -70,31 +70,13 @@
     <t>Nya medlemmar</t>
   </si>
   <si>
-    <t>Jonas Lind</t>
+    <t>Sofia Nilsson</t>
   </si>
   <si>
     <t>Domare</t>
   </si>
   <si>
     <t>Seriematch A</t>
-  </si>
-  <si>
-    <t>Projektstart</t>
-  </si>
-  <si>
-    <t>Filip Bäck</t>
-  </si>
-  <si>
-    <t>Utbildningsvecka</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Erik Dahl</t>
-  </si>
-  <si>
-    <t>Försäljning</t>
   </si>
 </sst>
 </file>
@@ -123,12 +105,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -141,16 +129,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -167,19 +155,19 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -199,6 +187,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -398,12 +387,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -435,10 +424,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -677,12 +666,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -986,10 +975,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1284,7 +1273,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="4">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E2" t="s" s="2">
         <v>11</v>
@@ -1293,7 +1282,7 @@
         <v>15</v>
       </c>
       <c r="G2" s="4">
-        <v>3750</v>
+        <v>120</v>
       </c>
       <c r="H2" t="s" s="2">
         <v>12</v>
@@ -1322,7 +1311,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="4">
-        <v>5600</v>
+        <v>300</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>15</v>
@@ -1351,7 +1340,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="4">
-        <v>2400</v>
+        <v>90</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>18</v>
@@ -1371,7 +1360,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="4">
-        <v>401</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s" s="2">
         <v>20</v>
@@ -1380,7 +1369,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="4">
-        <v>1800</v>
+        <v>100</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>21</v>
@@ -1390,120 +1379,48 @@
       </c>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3">
-        <v>45566</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4">
-        <v>402</v>
-      </c>
-      <c r="E6" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="F6" s="4">
-        <v>22</v>
-      </c>
-      <c r="G6" s="4">
-        <v>5500</v>
-      </c>
-      <c r="H6" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="I6" s="5">
-        <v>45600</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="B7" s="3">
-        <v>45566</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="D7" s="4">
-        <v>404</v>
-      </c>
-      <c r="E7" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="F7" s="4">
-        <v>7</v>
-      </c>
-      <c r="G7" s="4">
-        <v>9800</v>
-      </c>
-      <c r="H7" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="I7" s="5">
-        <v>45600</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3">
-        <v>45536</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4">
-        <v>403</v>
-      </c>
-      <c r="E8" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="F8" s="4">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4">
-        <v>2500</v>
-      </c>
-      <c r="H8" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="I8" s="5">
-        <v>45570</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3">
-        <v>45536</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="D9" s="4">
-        <v>404</v>
-      </c>
-      <c r="E9" t="s" s="2">
-        <v>17</v>
-      </c>
-      <c r="F9" s="4">
-        <v>8</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1600</v>
-      </c>
-      <c r="H9" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="I9" s="5">
-        <v>45570</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" s="6"/>

</xml_diff>